<commit_message>
getting data from excel
</commit_message>
<xml_diff>
--- a/restapicourse.xlsx
+++ b/restapicourse.xlsx
@@ -11,46 +11,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Testcases</t>
   </si>
   <si>
-    <t>header1</t>
-  </si>
-  <si>
-    <t>header2</t>
-  </si>
-  <si>
-    <t>header3</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>a22</t>
-  </si>
-  <si>
-    <t>a23</t>
-  </si>
-  <si>
-    <t>a24</t>
-  </si>
-  <si>
-    <t>Purchase</t>
-  </si>
-  <si>
-    <t>a32</t>
-  </si>
-  <si>
-    <t>a33</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>aisle</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>book1</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>isbn1</t>
+  </si>
+  <si>
+    <t>aisle1</t>
+  </si>
+  <si>
+    <t>author1</t>
+  </si>
+  <si>
+    <t>book2</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>isbn2</t>
+  </si>
+  <si>
+    <t>aisle2</t>
+  </si>
+  <si>
+    <t>author2</t>
+  </si>
+  <si>
+    <t>book3</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>isbn3</t>
+  </si>
+  <si>
+    <t>aisle3</t>
+  </si>
+  <si>
+    <t>author3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -60,6 +87,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -75,11 +103,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -302,42 +333,68 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
-        <v>34.0</v>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>